<commit_message>
Updated to fit full college names
</commit_message>
<xml_diff>
--- a/Sample.xlsx
+++ b/Sample.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="165">
   <si>
     <t>Division</t>
   </si>
@@ -422,6 +422,96 @@
   </si>
   <si>
     <t>York College (Pennsylvania)</t>
+  </si>
+  <si>
+    <t>Long Island University-Brooklyn Campus</t>
+  </si>
+  <si>
+    <t>North Carolina Central University</t>
+  </si>
+  <si>
+    <t>Southeastern Louisiana University</t>
+  </si>
+  <si>
+    <t>University of California, Berkeley</t>
+  </si>
+  <si>
+    <t>University of Massachusetts, Amherst</t>
+  </si>
+  <si>
+    <t>University of Missouri, Columbia</t>
+  </si>
+  <si>
+    <t>University of North Carolina Asheville</t>
+  </si>
+  <si>
+    <t>Albany State University (Georgia)</t>
+  </si>
+  <si>
+    <t>California State University, Monterey Bay</t>
+  </si>
+  <si>
+    <t>Georgia Southwestern State University</t>
+  </si>
+  <si>
+    <t>Kutztown University of Pennsylvania</t>
+  </si>
+  <si>
+    <t>Mansfield University of Pennsylvania</t>
+  </si>
+  <si>
+    <t>Metropolitan State University of Denver</t>
+  </si>
+  <si>
+    <t>Missouri Western State University</t>
+  </si>
+  <si>
+    <t>New Mexico Highlands University</t>
+  </si>
+  <si>
+    <t>Slippery Rock University of Pennsylvania</t>
+  </si>
+  <si>
+    <t>Texas A&amp;M International University</t>
+  </si>
+  <si>
+    <t>University of Minnesota, Crookston</t>
+  </si>
+  <si>
+    <t>University of Wisconsin-Parkside</t>
+  </si>
+  <si>
+    <t>Emmanuel College (Massachusetts)</t>
+  </si>
+  <si>
+    <t>Franciscan University of Steubenville</t>
+  </si>
+  <si>
+    <t>Massachusetts College of Liberal Arts</t>
+  </si>
+  <si>
+    <t>Saint Mary's University of Minnesota</t>
+  </si>
+  <si>
+    <t>St. Joseph's College (Long Island)</t>
+  </si>
+  <si>
+    <t>State University of New York at Geneseo</t>
+  </si>
+  <si>
+    <t>State University of New York at Oswego</t>
+  </si>
+  <si>
+    <t>State University of New York Maritime College</t>
+  </si>
+  <si>
+    <t>University of Mary Hardin-Baylor</t>
+  </si>
+  <si>
+    <t>Western Connecticut State University</t>
+  </si>
+  <si>
+    <t>William Paterson University of New Jersey</t>
   </si>
 </sst>
 </file>
@@ -760,7 +850,7 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
     <col min="3" max="3" width="13" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
     <col min="5" max="5" width="13" customWidth="1"/>
@@ -1094,7 +1184,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>20</v>
+        <v>135</v>
       </c>
       <c r="C12">
         <v>351</v>
@@ -1297,7 +1387,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>27</v>
+        <v>136</v>
       </c>
       <c r="C19">
         <v>351</v>
@@ -1413,7 +1503,7 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>137</v>
       </c>
       <c r="C23">
         <v>351</v>
@@ -1529,7 +1619,7 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>35</v>
+        <v>138</v>
       </c>
       <c r="C27">
         <v>351</v>
@@ -1674,7 +1764,7 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>40</v>
+        <v>139</v>
       </c>
       <c r="C32">
         <v>351</v>
@@ -1703,7 +1793,7 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>41</v>
+        <v>140</v>
       </c>
       <c r="C33">
         <v>351</v>
@@ -1732,7 +1822,7 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>141</v>
       </c>
       <c r="C34">
         <v>351</v>
@@ -1935,7 +2025,7 @@
         <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>50</v>
+        <v>142</v>
       </c>
       <c r="C41">
         <v>314</v>
@@ -2138,7 +2228,7 @@
         <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>57</v>
+        <v>143</v>
       </c>
       <c r="C48">
         <v>314</v>
@@ -2370,7 +2460,7 @@
         <v>2</v>
       </c>
       <c r="B56" t="s">
-        <v>65</v>
+        <v>144</v>
       </c>
       <c r="C56">
         <v>314</v>
@@ -2399,7 +2489,7 @@
         <v>2</v>
       </c>
       <c r="B57" t="s">
-        <v>66</v>
+        <v>145</v>
       </c>
       <c r="C57">
         <v>314</v>
@@ -2486,7 +2576,7 @@
         <v>2</v>
       </c>
       <c r="B60" t="s">
-        <v>69</v>
+        <v>146</v>
       </c>
       <c r="C60">
         <v>314</v>
@@ -2515,7 +2605,7 @@
         <v>2</v>
       </c>
       <c r="B61" t="s">
-        <v>70</v>
+        <v>147</v>
       </c>
       <c r="C61">
         <v>314</v>
@@ -2544,7 +2634,7 @@
         <v>2</v>
       </c>
       <c r="B62" t="s">
-        <v>71</v>
+        <v>148</v>
       </c>
       <c r="C62">
         <v>314</v>
@@ -2573,7 +2663,7 @@
         <v>2</v>
       </c>
       <c r="B63" t="s">
-        <v>72</v>
+        <v>149</v>
       </c>
       <c r="C63">
         <v>314</v>
@@ -2689,7 +2779,7 @@
         <v>2</v>
       </c>
       <c r="B67" t="s">
-        <v>77</v>
+        <v>150</v>
       </c>
       <c r="C67">
         <v>314</v>
@@ -2718,7 +2808,7 @@
         <v>2</v>
       </c>
       <c r="B68" t="s">
-        <v>78</v>
+        <v>151</v>
       </c>
       <c r="C68">
         <v>314</v>
@@ -2834,7 +2924,7 @@
         <v>2</v>
       </c>
       <c r="B72" t="s">
-        <v>82</v>
+        <v>152</v>
       </c>
       <c r="C72">
         <v>314</v>
@@ -2892,7 +2982,7 @@
         <v>2</v>
       </c>
       <c r="B74" t="s">
-        <v>84</v>
+        <v>153</v>
       </c>
       <c r="C74">
         <v>314</v>
@@ -3153,7 +3243,7 @@
         <v>3</v>
       </c>
       <c r="B83" t="s">
-        <v>93</v>
+        <v>154</v>
       </c>
       <c r="C83">
         <v>440</v>
@@ -3269,7 +3359,7 @@
         <v>3</v>
       </c>
       <c r="B87" t="s">
-        <v>97</v>
+        <v>155</v>
       </c>
       <c r="C87">
         <v>440</v>
@@ -3414,7 +3504,7 @@
         <v>3</v>
       </c>
       <c r="B92" t="s">
-        <v>102</v>
+        <v>156</v>
       </c>
       <c r="C92">
         <v>440</v>
@@ -3704,7 +3794,7 @@
         <v>3</v>
       </c>
       <c r="B102" t="s">
-        <v>113</v>
+        <v>157</v>
       </c>
       <c r="C102">
         <v>440</v>
@@ -3791,7 +3881,7 @@
         <v>3</v>
       </c>
       <c r="B105" t="s">
-        <v>116</v>
+        <v>158</v>
       </c>
       <c r="C105">
         <v>440</v>
@@ -3820,7 +3910,7 @@
         <v>3</v>
       </c>
       <c r="B106" t="s">
-        <v>117</v>
+        <v>159</v>
       </c>
       <c r="C106">
         <v>440</v>
@@ -3849,7 +3939,7 @@
         <v>3</v>
       </c>
       <c r="B107" t="s">
-        <v>117</v>
+        <v>160</v>
       </c>
       <c r="C107">
         <v>440</v>
@@ -3878,7 +3968,7 @@
         <v>3</v>
       </c>
       <c r="B108" t="s">
-        <v>118</v>
+        <v>161</v>
       </c>
       <c r="C108">
         <v>440</v>
@@ -4023,7 +4113,7 @@
         <v>3</v>
       </c>
       <c r="B113" t="s">
-        <v>123</v>
+        <v>162</v>
       </c>
       <c r="C113">
         <v>440</v>
@@ -4255,7 +4345,7 @@
         <v>3</v>
       </c>
       <c r="B121" t="s">
-        <v>131</v>
+        <v>163</v>
       </c>
       <c r="C121">
         <v>440</v>
@@ -4284,7 +4374,7 @@
         <v>3</v>
       </c>
       <c r="B122" t="s">
-        <v>132</v>
+        <v>164</v>
       </c>
       <c r="C122">
         <v>440</v>

</xml_diff>

<commit_message>
Update again, incorrect files uploaded last time
</commit_message>
<xml_diff>
--- a/Sample.xlsx
+++ b/Sample.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="136">
   <si>
     <t>Division</t>
   </si>
@@ -79,7 +79,7 @@
     <t>Lipscomb University</t>
   </si>
   <si>
-    <t>Long Island University-Brookly</t>
+    <t>Long Island University-Brooklyn Campus</t>
   </si>
   <si>
     <t>Louisiana Tech University</t>
@@ -100,7 +100,7 @@
     <t>Murray State University</t>
   </si>
   <si>
-    <t>North Carolina Central Univers</t>
+    <t>North Carolina Central University</t>
   </si>
   <si>
     <t>Northern Illinois University</t>
@@ -112,7 +112,7 @@
     <t>Portland State University</t>
   </si>
   <si>
-    <t>Southeastern Louisiana Univers</t>
+    <t>Southeastern Louisiana University</t>
   </si>
   <si>
     <t>St. Bonaventure University</t>
@@ -124,7 +124,7 @@
     <t>University of Arizona</t>
   </si>
   <si>
-    <t>University of California, Berk</t>
+    <t>University of California, Berkeley</t>
   </si>
   <si>
     <t>University of Detroit Mercy</t>
@@ -139,16 +139,16 @@
     <t>University of Hawaii, Manoa</t>
   </si>
   <si>
-    <t>University of Massachusetts, A</t>
-  </si>
-  <si>
-    <t>University of Missouri, Columb</t>
+    <t>University of Massachusetts, Amherst</t>
+  </si>
+  <si>
+    <t>University of Missouri, Columbia</t>
   </si>
   <si>
     <t>Alice</t>
   </si>
   <si>
-    <t>University of North Carolina A</t>
+    <t>University of North Carolina Asheville</t>
   </si>
   <si>
     <t>University of Pennsylvania</t>
@@ -169,7 +169,7 @@
     <t>Wofford College</t>
   </si>
   <si>
-    <t>Albany State University (Georg</t>
+    <t>Albany State University (Georgia)</t>
   </si>
   <si>
     <t>Assumption College</t>
@@ -190,7 +190,7 @@
     <t>Bowie State University</t>
   </si>
   <si>
-    <t>California State University, M</t>
+    <t>California State University, Monterey Bay</t>
   </si>
   <si>
     <t>Catawba College</t>
@@ -214,10 +214,10 @@
     <t>Gannon University</t>
   </si>
   <si>
-    <t>Georgia Southwestern State Uni</t>
-  </si>
-  <si>
-    <t>Kutztown University of Pennsyl</t>
+    <t>Georgia Southwestern State University</t>
+  </si>
+  <si>
+    <t>Kutztown University of Pennsylvania</t>
   </si>
   <si>
     <t>Lenoir-Rhyne University</t>
@@ -226,16 +226,16 @@
     <t>Lubbock Christian University</t>
   </si>
   <si>
-    <t>Mansfield University of Pennsy</t>
-  </si>
-  <si>
-    <t>Metropolitan State University</t>
-  </si>
-  <si>
-    <t>Missouri Western State Univers</t>
-  </si>
-  <si>
-    <t>New Mexico Highlands Universit</t>
+    <t>Mansfield University of Pennsylvania</t>
+  </si>
+  <si>
+    <t>Metropolitan State University of Denver</t>
+  </si>
+  <si>
+    <t>Missouri Western State University</t>
+  </si>
+  <si>
+    <t>New Mexico Highlands University</t>
   </si>
   <si>
     <t>North Greenville University</t>
@@ -250,10 +250,10 @@
     <t>Shaw University</t>
   </si>
   <si>
-    <t>Slippery Rock University of Pe</t>
-  </si>
-  <si>
-    <t>Texas A&amp;M International Univer</t>
+    <t>Slippery Rock University of Pennsylvania</t>
+  </si>
+  <si>
+    <t>Texas A&amp;M International University</t>
   </si>
   <si>
     <t>Texas Woman's University</t>
@@ -265,13 +265,13 @@
     <t>University of Central Missouri</t>
   </si>
   <si>
-    <t>University of Minnesota, Crook</t>
+    <t>University of Minnesota, Crookston</t>
   </si>
   <si>
     <t>University of Mount Olive</t>
   </si>
   <si>
-    <t>University of Wisconsin-Parksi</t>
+    <t>University of Wisconsin-Parkside</t>
   </si>
   <si>
     <t>Westminster College (Utah)</t>
@@ -298,7 +298,7 @@
     <t>Elmira College</t>
   </si>
   <si>
-    <t>Emmanuel College (Massachusett</t>
+    <t>Emmanuel College (Massachusetts)</t>
   </si>
   <si>
     <t>Emory University</t>
@@ -310,7 +310,7 @@
     <t>Fontbonne University</t>
   </si>
   <si>
-    <t>Franciscan University of Steub</t>
+    <t>Franciscan University of Steubenville</t>
   </si>
   <si>
     <t>Hampden-Sydney College</t>
@@ -325,7 +325,7 @@
     <t>Maranatha Baptist University</t>
   </si>
   <si>
-    <t>Massachusetts College of Liber</t>
+    <t>Massachusetts College of Liberal Arts</t>
   </si>
   <si>
     <t>McMurry University</t>
@@ -358,7 +358,7 @@
     <t>Ripon College</t>
   </si>
   <si>
-    <t>Saint Mary's University of Min</t>
+    <t>Saint Mary's University of Minnesota</t>
   </si>
   <si>
     <t>Salisbury University</t>
@@ -367,13 +367,16 @@
     <t>Southern Virginia University</t>
   </si>
   <si>
-    <t>St. Joseph's College (Long Isl</t>
-  </si>
-  <si>
-    <t>State University of New York a</t>
-  </si>
-  <si>
-    <t>State University of New York M</t>
+    <t>St. Joseph's College (Long Island)</t>
+  </si>
+  <si>
+    <t>State University of New York at Geneseo</t>
+  </si>
+  <si>
+    <t>State University of New York at Oswego</t>
+  </si>
+  <si>
+    <t>State University of New York Maritime College</t>
   </si>
   <si>
     <t>Thomas More College</t>
@@ -388,7 +391,7 @@
     <t>Tufts University</t>
   </si>
   <si>
-    <t>University of Mary Hardin-Bayl</t>
+    <t>University of Mary Hardin-Baylor</t>
   </si>
   <si>
     <t>University of Rochester</t>
@@ -412,106 +415,16 @@
     <t>Wesley College</t>
   </si>
   <si>
-    <t>Western Connecticut State Univ</t>
-  </si>
-  <si>
-    <t>William Paterson University of</t>
+    <t>Western Connecticut State University</t>
+  </si>
+  <si>
+    <t>William Paterson University of New Jersey</t>
   </si>
   <si>
     <t>Yeshiva University</t>
   </si>
   <si>
     <t>York College (Pennsylvania)</t>
-  </si>
-  <si>
-    <t>Long Island University-Brooklyn Campus</t>
-  </si>
-  <si>
-    <t>North Carolina Central University</t>
-  </si>
-  <si>
-    <t>Southeastern Louisiana University</t>
-  </si>
-  <si>
-    <t>University of California, Berkeley</t>
-  </si>
-  <si>
-    <t>University of Massachusetts, Amherst</t>
-  </si>
-  <si>
-    <t>University of Missouri, Columbia</t>
-  </si>
-  <si>
-    <t>University of North Carolina Asheville</t>
-  </si>
-  <si>
-    <t>Albany State University (Georgia)</t>
-  </si>
-  <si>
-    <t>California State University, Monterey Bay</t>
-  </si>
-  <si>
-    <t>Georgia Southwestern State University</t>
-  </si>
-  <si>
-    <t>Kutztown University of Pennsylvania</t>
-  </si>
-  <si>
-    <t>Mansfield University of Pennsylvania</t>
-  </si>
-  <si>
-    <t>Metropolitan State University of Denver</t>
-  </si>
-  <si>
-    <t>Missouri Western State University</t>
-  </si>
-  <si>
-    <t>New Mexico Highlands University</t>
-  </si>
-  <si>
-    <t>Slippery Rock University of Pennsylvania</t>
-  </si>
-  <si>
-    <t>Texas A&amp;M International University</t>
-  </si>
-  <si>
-    <t>University of Minnesota, Crookston</t>
-  </si>
-  <si>
-    <t>University of Wisconsin-Parkside</t>
-  </si>
-  <si>
-    <t>Emmanuel College (Massachusetts)</t>
-  </si>
-  <si>
-    <t>Franciscan University of Steubenville</t>
-  </si>
-  <si>
-    <t>Massachusetts College of Liberal Arts</t>
-  </si>
-  <si>
-    <t>Saint Mary's University of Minnesota</t>
-  </si>
-  <si>
-    <t>St. Joseph's College (Long Island)</t>
-  </si>
-  <si>
-    <t>State University of New York at Geneseo</t>
-  </si>
-  <si>
-    <t>State University of New York at Oswego</t>
-  </si>
-  <si>
-    <t>State University of New York Maritime College</t>
-  </si>
-  <si>
-    <t>University of Mary Hardin-Baylor</t>
-  </si>
-  <si>
-    <t>Western Connecticut State University</t>
-  </si>
-  <si>
-    <t>William Paterson University of New Jersey</t>
   </si>
 </sst>
 </file>
@@ -1184,7 +1097,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>135</v>
+        <v>20</v>
       </c>
       <c r="C12">
         <v>351</v>
@@ -1387,7 +1300,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>136</v>
+        <v>27</v>
       </c>
       <c r="C19">
         <v>351</v>
@@ -1503,7 +1416,7 @@
         <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>137</v>
+        <v>31</v>
       </c>
       <c r="C23">
         <v>351</v>
@@ -1619,7 +1532,7 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>138</v>
+        <v>35</v>
       </c>
       <c r="C27">
         <v>351</v>
@@ -1764,7 +1677,7 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>139</v>
+        <v>40</v>
       </c>
       <c r="C32">
         <v>351</v>
@@ -1793,7 +1706,7 @@
         <v>1</v>
       </c>
       <c r="B33" t="s">
-        <v>140</v>
+        <v>41</v>
       </c>
       <c r="C33">
         <v>351</v>
@@ -1822,7 +1735,7 @@
         <v>1</v>
       </c>
       <c r="B34" t="s">
-        <v>141</v>
+        <v>43</v>
       </c>
       <c r="C34">
         <v>351</v>
@@ -2025,7 +1938,7 @@
         <v>2</v>
       </c>
       <c r="B41" t="s">
-        <v>142</v>
+        <v>50</v>
       </c>
       <c r="C41">
         <v>314</v>
@@ -2228,7 +2141,7 @@
         <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>143</v>
+        <v>57</v>
       </c>
       <c r="C48">
         <v>314</v>
@@ -2460,7 +2373,7 @@
         <v>2</v>
       </c>
       <c r="B56" t="s">
-        <v>144</v>
+        <v>65</v>
       </c>
       <c r="C56">
         <v>314</v>
@@ -2489,7 +2402,7 @@
         <v>2</v>
       </c>
       <c r="B57" t="s">
-        <v>145</v>
+        <v>66</v>
       </c>
       <c r="C57">
         <v>314</v>
@@ -2576,7 +2489,7 @@
         <v>2</v>
       </c>
       <c r="B60" t="s">
-        <v>146</v>
+        <v>69</v>
       </c>
       <c r="C60">
         <v>314</v>
@@ -2605,7 +2518,7 @@
         <v>2</v>
       </c>
       <c r="B61" t="s">
-        <v>147</v>
+        <v>70</v>
       </c>
       <c r="C61">
         <v>314</v>
@@ -2634,7 +2547,7 @@
         <v>2</v>
       </c>
       <c r="B62" t="s">
-        <v>148</v>
+        <v>71</v>
       </c>
       <c r="C62">
         <v>314</v>
@@ -2663,7 +2576,7 @@
         <v>2</v>
       </c>
       <c r="B63" t="s">
-        <v>149</v>
+        <v>72</v>
       </c>
       <c r="C63">
         <v>314</v>
@@ -2779,7 +2692,7 @@
         <v>2</v>
       </c>
       <c r="B67" t="s">
-        <v>150</v>
+        <v>77</v>
       </c>
       <c r="C67">
         <v>314</v>
@@ -2808,7 +2721,7 @@
         <v>2</v>
       </c>
       <c r="B68" t="s">
-        <v>151</v>
+        <v>78</v>
       </c>
       <c r="C68">
         <v>314</v>
@@ -2924,7 +2837,7 @@
         <v>2</v>
       </c>
       <c r="B72" t="s">
-        <v>152</v>
+        <v>82</v>
       </c>
       <c r="C72">
         <v>314</v>
@@ -2982,7 +2895,7 @@
         <v>2</v>
       </c>
       <c r="B74" t="s">
-        <v>153</v>
+        <v>84</v>
       </c>
       <c r="C74">
         <v>314</v>
@@ -3243,7 +3156,7 @@
         <v>3</v>
       </c>
       <c r="B83" t="s">
-        <v>154</v>
+        <v>93</v>
       </c>
       <c r="C83">
         <v>440</v>
@@ -3359,7 +3272,7 @@
         <v>3</v>
       </c>
       <c r="B87" t="s">
-        <v>155</v>
+        <v>97</v>
       </c>
       <c r="C87">
         <v>440</v>
@@ -3504,7 +3417,7 @@
         <v>3</v>
       </c>
       <c r="B92" t="s">
-        <v>156</v>
+        <v>102</v>
       </c>
       <c r="C92">
         <v>440</v>
@@ -3794,7 +3707,7 @@
         <v>3</v>
       </c>
       <c r="B102" t="s">
-        <v>157</v>
+        <v>113</v>
       </c>
       <c r="C102">
         <v>440</v>
@@ -3881,7 +3794,7 @@
         <v>3</v>
       </c>
       <c r="B105" t="s">
-        <v>158</v>
+        <v>116</v>
       </c>
       <c r="C105">
         <v>440</v>
@@ -3910,7 +3823,7 @@
         <v>3</v>
       </c>
       <c r="B106" t="s">
-        <v>159</v>
+        <v>117</v>
       </c>
       <c r="C106">
         <v>440</v>
@@ -3939,7 +3852,7 @@
         <v>3</v>
       </c>
       <c r="B107" t="s">
-        <v>160</v>
+        <v>118</v>
       </c>
       <c r="C107">
         <v>440</v>
@@ -3968,7 +3881,7 @@
         <v>3</v>
       </c>
       <c r="B108" t="s">
-        <v>161</v>
+        <v>119</v>
       </c>
       <c r="C108">
         <v>440</v>
@@ -3997,7 +3910,7 @@
         <v>3</v>
       </c>
       <c r="B109" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="C109">
         <v>440</v>
@@ -4026,7 +3939,7 @@
         <v>3</v>
       </c>
       <c r="B110" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C110">
         <v>440</v>
@@ -4055,7 +3968,7 @@
         <v>3</v>
       </c>
       <c r="B111" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C111">
         <v>440</v>
@@ -4084,7 +3997,7 @@
         <v>3</v>
       </c>
       <c r="B112" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C112">
         <v>440</v>
@@ -4113,7 +4026,7 @@
         <v>3</v>
       </c>
       <c r="B113" t="s">
-        <v>162</v>
+        <v>124</v>
       </c>
       <c r="C113">
         <v>440</v>
@@ -4142,7 +4055,7 @@
         <v>3</v>
       </c>
       <c r="B114" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C114">
         <v>440</v>
@@ -4171,7 +4084,7 @@
         <v>3</v>
       </c>
       <c r="B115" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C115">
         <v>440</v>
@@ -4200,7 +4113,7 @@
         <v>3</v>
       </c>
       <c r="B116" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C116">
         <v>440</v>
@@ -4229,7 +4142,7 @@
         <v>3</v>
       </c>
       <c r="B117" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="C117">
         <v>440</v>
@@ -4258,7 +4171,7 @@
         <v>3</v>
       </c>
       <c r="B118" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="C118">
         <v>440</v>
@@ -4287,7 +4200,7 @@
         <v>3</v>
       </c>
       <c r="B119" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C119">
         <v>440</v>
@@ -4316,7 +4229,7 @@
         <v>3</v>
       </c>
       <c r="B120" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="C120">
         <v>440</v>
@@ -4345,7 +4258,7 @@
         <v>3</v>
       </c>
       <c r="B121" t="s">
-        <v>163</v>
+        <v>132</v>
       </c>
       <c r="C121">
         <v>440</v>
@@ -4374,7 +4287,7 @@
         <v>3</v>
       </c>
       <c r="B122" t="s">
-        <v>164</v>
+        <v>133</v>
       </c>
       <c r="C122">
         <v>440</v>
@@ -4403,7 +4316,7 @@
         <v>3</v>
       </c>
       <c r="B123" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C123">
         <v>440</v>
@@ -4432,7 +4345,7 @@
         <v>3</v>
       </c>
       <c r="B124" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C124">
         <v>440</v>

</xml_diff>